<commit_message>
Adicionando introdução aos fundos e corrigindo tamanho da fonte e nomes dos graficos
</commit_message>
<xml_diff>
--- a/data-raw/resenhas/fundos.xlsx
+++ b/data-raw/resenhas/fundos.xlsx
@@ -62,38 +62,72 @@
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, que tenham como objetivo aplicar seus recursos em ações de empresas, dispostos a assumir os riscos e as estratégias de investimento do fundo, em especial quanto às variações no mercado de ações.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas, por meio de aplicação em cotas do BTG Pactual Dividendos Fundo de Investimento em cotas de fundos de investimento em ações (fundo investido), além de outros ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, sem perseguir uma correlação com qualquer índice de ações ou benchmark específico, não constituindo, em hipótese alguma, garantia ou promessa de rentabilidade por parte do administrador e/ou gestor.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                        &lt;b&gt;Classificação CVM: Ações&lt;/b&gt;&lt;br&gt;                                                                       &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                                                       &lt;b&gt;Resgate: D + 5 dias úteis&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 2,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 15:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
  O fundo é destinado à captação de recursos de investidores pessoas físicas, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
 &lt;br&gt;&lt;br&gt;
 &lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como fundo de investimento em cotas de fundos de investimento Multimercado e investirá, no mínimo, 95% (noventa e cinco por cento) de seu patrimônio líquido em cotas de fundos de investimento cuja política de investimento consista em aplicar seus recursos, preponderantemente, em debêntures de infraestrutura que atendam aos critérios de elegibilidade previstos na Lei nº 12.431 de 24 de junho de 2011 (“Ativos de Infraestrutura” e “Lei 12.431/11”, respectivamente), que venham a ser selecionados pela gestora e que atendam os requisitos deste Regulamento, podendo utilizar estratégias nos mercados de títulos públicos, derivativos e títulos privados, além de outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, buscando proporcionar aos seus cotistas retorno de capital no longo prazo, sem perseguir uma correlação com qualquer índice ou benchmark específico.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                            &lt;b&gt;Classificação CVM: Multimercado &lt;/b&gt;&lt;br&gt;                                                                                                                          &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 5 dias úteis&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 1,15 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 13:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-Destina-se à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, que tenham como objetivo aplicar seus recursos em ações de empresas, dispostos a assumir os riscos e as estratégias de investimento do fundo, em especial quanto às variações no mercado de ações.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como fundo de investimento em cotas de fundos de investimento de ações e investirá, no mínimo, 95% (noventa e cinco por cento) de seu patrimônio líquido em cotas do BTG Pactual Absoluto Institucional Fundo de Investimento em cotas de fundos de investimento de ações, inscrito no CNPJ sob o nº 11.977.794/0001-64, doravante designado fundo de investimento além de outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, sem perseguir uma correlação com qualquer índice de ações ou benchmark específico. O fundo e os fundos de investimento no qual este investe, podem estar expostos à significativa concentração em ativos financeiros de poucos emissores, com os riscos daí decorrentes.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                        &lt;b&gt;Classificação CVM: Ações&lt;/b&gt;&lt;br&gt;                                                                       &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                                                       &lt;b&gt;Resgate: D + 5 dias úteis&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 2,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 15:00h&lt;/b&gt;&lt;br&gt;</t>
+O fundo é classificado como fundo de investimento em cotas de fundos de investimento Multimercado e investirá, no mínimo, 95% (noventa e cinco por cento) de seu patrimônio líquido em cotas de fundos de investimento cuja política de investimento consista em aplicar seus recursos, preponderantemente, em debêntures de infraestrutura que atendam aos critérios de elegibilidade previstos na Lei nº 12.431 de 24 de junho de 2011 (“Ativos de Infraestrutura” e “Lei 12.431/11”, respectivamente), que venham a ser selecionados pela gestora e que atendam os requisitos deste Regulamento, podendo utilizar estratégias nos mercados de títulos públicos, derivativos e títulos privados, além de outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, buscando proporcionar aos seus cotistas retorno de capital no longo prazo, sem perseguir uma correlação com qualquer índice ou benchmark específico.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                            &lt;b&gt;Classificação CVM: Multimercado &lt;/b&gt;&lt;br&gt;                                                                                                                          &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 5 dias úteis&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 1,15 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 13:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+Destina-se à captação de recursos de investidores pessoas físicas e jurídicas, inclusive fundos de investimento que tenham como objetivo aplicar seus recursos em ações de empresas, cientes dos riscos inerentes ao mercado acionário.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como fundo de investimento em cotas de fundos de investimento de ações e investirá, no mínimo, 95% (noventa e cinco por cento) de seu patrimônio líquido em cotas do BTG Pactual Absoluto Institucional Fundo de Investimento em cotas de fundos de investimento de ações, inscrito no CNPJ sob o nº 11.977.794/0001-64, doravante designado fundo de investimento além de outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, sem perseguir uma correlação com qualquer índice de ações ou benchmark específico. O fundo e os fundos de investimento no qual este investe, podem estar expostos à significativa concentração em ativos financeiros de poucos emissores, com os riscos daí decorrentes.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                        &lt;b&gt;Classificação CVM: Ações&lt;/b&gt;&lt;br&gt;                                                                       &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                                                       &lt;b&gt;Resgate: D + 30 dias corridos&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 3,00 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 15:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O fundo é destinado à captação de recursos das Entidades Fechadas de Previdência Privada Complementar (EFPC), dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, das Companhias Seguradoras e de Fundos de Investimento e de Fundos de Investimento em Cotas de Fundos de Investimento, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista. O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas por meio da aplicação dos recursos da sua carteira em títulos públicos federais indexados a taxas de juros prefixadas e/ou pós-fixadas (SELIC/CDI), não constituindo, em qualquer hipótese, garantia ou promessa de rentabilidade por parte do administrador.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração. Para alcançar seus objetivos, o fundo aplicará seus recursos exclusivamente em títulos de emissão do Tesouro Nacional, registrados no Sistema Especial de Liquidação e Custódia (SELIC) ou operações compromissadas lastreadas nestes títulos.
+O prazo médio da carteira do fundo será de até 365 (trezentos e sessenta e cinco dias). A carteira do fundo deverá ter como parâmetro de rentabilidade o subíndice IRF-M 1 da ANBIMA          &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 1&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,15% a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: 16:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O Fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.             &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,80 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
 O Fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador, doravante designados, coletivamente, cotistas ou, individualmente, cotista
 &lt;br&gt;&lt;br&gt;
 &lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo  é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.            &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 500,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 1,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
+O fundo  é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.            &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 500,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 1,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O Fundo é é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo  é classificado como Renda Fixa Referenciado DI e seus recursos serão aplicados em ativos financeiros que buscam acompanhar a variação do Certificado de Depósito Interbancário (CDI) ou da taxa SELIC, de forma que, no mínimo, 95% (noventa e cinco por cento) dos ativos financeiros componentes de sua carteira estejam atrelados a este parâmetro, direta ou indiretamente, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração.                &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 500.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,20 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: 17:30h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O Fundo é destinado à captação de recursos das Entidades Fechadas de Previdência Complementar (EFPC), dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração.
+Para alcançar seus objetivos, o fundo aplicará seus recursos exclusivamente em títulos de emissão do Tesouro Nacional, registrados no Sistema Especial de Liquidação e Custódia (SELIC) e/ou operações compromissadas lastreadas nesses títulos.
+A carteira do fundo deverá ter como parâmetro de rentabilidade o subíndice IMA-B da ANBIMA.                                                                     &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0*&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,20% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 16:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
-O fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador, doravante designados, coletivamente, cotistas ou, individualmente, cotista.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento, devendo observar o limite mínimo de 80% (oitenta por cento) de seu patrimônio, isolada ou cumulativamente, em: a - títulos da dívida pública federal; e b - ativos financeiros de renda fixa considerados de baixo risco de crédito pelo gestor.                                        &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;     &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                            &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,5% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 16:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O Fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios. Tem por objetivo proporcionar aos seus cotistas rentabilidade através de investimentos em cotas de fundos de investimento classificados como “Renda Fixa”, os quais apliquem, no mínimo, 80% (oitenta por cento) de seus recursos em ativos financeiros relacionados diretamente, ou sintetizados via derivativos, ao fator de risco que dá nome à classe
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento..                                   &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;&lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                             &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 1&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,50% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
+Destina-se exclusivamente à captação de recursos de investidores isentos de Imposto de Renda, - IR e Imposto Sobre Operações Financeiras - IOF, principalmente dos setores públicos estadual e municipal que busquem um aumento do capital investido com um risco de investimento inerente às aplicações de mercado de renda fixa, com liquidez diária e a comodidade de resgate/aplicação automático.
+Para o cliente obter o benefício da aplicação ou resgate automático, é necessário fazer o cadastramento prévio na agência onde possui conta corrente.
+O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas por meio de aplicação dos recursos em títulos e valores mobiliários, demais ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definidos pela legislação em vigor e por seu regulamento, não constituindo, por parte do administrador garantia ou promessa de rentabilidade. O indexador é utilizado somente como referência para comparativo da rentabilidade e não como parâmetro para objetivo do fundo
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundoé classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.
+&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 1,70% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
@@ -102,14 +136,35 @@
 O objetivo do Fundo de Investimento Banestes Solidez Automático é possibilitar aos seus cotistas valorização de suas cotas resultantes da administração criteriosa e racional da carteira do Fundo.
 &lt;br&gt;&lt;br&gt;
 &lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo  é classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.                                   &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 0&lt;/b&gt;&lt;br&gt;&lt;b&gt;Classificação CVM: Renda Fixa Curto Prazo&lt;/b&gt;&lt;br&gt;                                                                             &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,5% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
+O fundo  é classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.                                   &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 0&lt;/b&gt;&lt;br&gt;&lt;b&gt;Classificação CVM: Renda Fixa Curto Prazo&lt;/b&gt;&lt;br&gt;                                                                             &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,5% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
 O fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento e de Fundos de Investimento em Cotas de Fundos de Investimento, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
 &lt;br&gt;&lt;br&gt;
 &lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais. Os recursos do fundo serão aplicados exclusivamente em Títulos Públicos Federais, indexados a taxas pós fixadas (SELIC/CDI) e/ou índice de preços e/ou pré-fixadas em operações finais e/ou compromissadas lastreadas em títulos públicos, registrados no Sistema Especial de Liquidação e Custódia (SELIC).                                                                                &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 1.000,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 1% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 16:00h&lt;/b&gt;&lt;br&gt;</t>
+O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais. Os recursos do fundo serão aplicados exclusivamente em Títulos Públicos Federais, indexados a taxas pós fixadas (SELIC/CDI) e/ou índice de preços e/ou pré-fixadas em operações finais e/ou compromissadas lastreadas em títulos públicos, registrados no Sistema Especial de Liquidação e Custódia (SELIC).                                                                                &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 1.000,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 1% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 16:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O Fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios. Tem por objetivo proporcionar aos seus cotistas rentabilidade através de investimentos em cotas de fundos de investimento classificados como “Renda Fixa”, os quais apliquem, no mínimo, 80% (oitenta por cento) de seus recursos em ativos financeiros relacionados diretamente, ou sintetizados via derivativos, ao fator de risco que dá nome à classe
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.                                   &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;&lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                             &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 2&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,50% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
+O Fundo  é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, dispostos a assumir os riscos e as estratégias de investimento do fundo, em especial quanto ás variações da taxa de juros.  O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas, próxima ao CDI (taxa média praticada por instituições financeiras), por meio de aplicação dos recursos em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definidos pela legislação em vigor, não constituindo, em hipótese alguma, garantia ou promessa de rentabilidade por parte do administrador e/ou do gestor.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.           &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
+O fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador, doravante designados, coletivamente, cotistas ou, individualmente, cotista.
+&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
+O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento, devendo observar o limite mínimo de 80% (oitenta por cento) de seu patrimônio, isolada ou cumulativamente, em: a - títulos da dívida pública federal; e b - ativos financeiros de renda fixa considerados de baixo risco de crédito pelo gestor.                                        &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;     &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                            &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 0,20% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 16:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
@@ -118,62 +173,7 @@
 O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas por meio de aplicação dos recursos em títulos e valores mobiliários, demais ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definidos pela legislação em vigor e por seu regulamento. O indexador é utilizado somente como referência para comparativo da rentabilidade e não como parâmetro para objetivo do fundo.
 &lt;br&gt;&lt;br&gt;
 &lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.                                                               &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa Curto Prazo&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0*&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 1,7% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;
-Destina-se exclusivamente à captação de recursos de investidores isentos de Imposto de Renda, - IR e Imposto Sobre Operações Financeiras - IOF, principalmente dos setores públicos estadual e municipal que busquem um aumento do capital investido com um risco de investimento inerente às aplicações de mercado de renda fixa, com liquidez diária e a comodidade de resgate/aplicação automático.
-Para o cliente obter o benefício da aplicação ou resgate automático, é necessário fazer o cadastramento prévio na agência onde possui conta corrente.
-O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas por meio de aplicação dos recursos em títulos e valores mobiliários, demais ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, conforme definidos pela legislação em vigor e por seu regulamento, não constituindo, por parte do administrador garantia ou promessa de rentabilidade. O indexador é utilizado somente como referência para comparativo da rentabilidade e não como parâmetro para objetivo do fundo
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundoé classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.
-&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 1,70% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O Fundo é destinado à captação de recursos das Entidades Fechadas de Previdência Complementar (EFPC), dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração.
-Para alcançar seus objetivos, o fundo aplicará seus recursos exclusivamente em títulos de emissão do Tesouro Nacional, registrados no Sistema Especial de Liquidação e Custódia (SELIC) e/ou operações compromissadas lastreadas nesses títulos.
-A carteira do fundo deverá ter como parâmetro de rentabilidade o subíndice IMA-B da ANBIMA.                                                                     &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Médio&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0*&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,20% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 16:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O Fundo é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.             &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,80 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O Fundo é é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo  é classificado como Renda Fixa Referenciado DI e seus recursos serão aplicados em ativos financeiros que buscam acompanhar a variação do Certificado de Depósito Interbancário (CDI) ou da taxa SELIC, de forma que, no mínimo, 95% (noventa e cinco por cento) dos ativos financeiros componentes de sua carteira estejam atrelados a este parâmetro, direta ou indiretamente, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração.                &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 500.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,20 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:30h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-Destina-se à captação de recursos de investidores pessoas físicas e jurídicas, inclusive fundos de investimento que tenham como objetivo aplicar seus recursos em ações de empresas, cientes dos riscos inerentes ao mercado acionário.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como fundo de investimento em cotas de fundos de investimento de ações e investirá, no mínimo, 95% (noventa e cinco por cento) de seu patrimônio líquido em cotas do BTG Pactual Absoluto Institucional Fundo de Investimento em cotas de fundos de investimento de ações, inscrito no CNPJ sob o nº 11.977.794/0001-64, doravante designado fundo de investimento além de outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, sem perseguir uma correlação com qualquer índice de ações ou benchmark específico. O fundo e os fundos de investimento no qual este investe, podem estar expostos à significativa concentração em ativos financeiros de poucos emissores, com os riscos daí decorrentes.&lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 5.000,00&lt;/b&gt;&lt;br&gt;                                                        &lt;b&gt;Classificação CVM: Ações&lt;/b&gt;&lt;br&gt;                                                                       &lt;b&gt;Classificação de risco: Alto &lt;/b&gt;&lt;br&gt;                                                                                                       &lt;b&gt;Resgate: D + 30 dias corridos&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 3,00 % a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: Até às 15:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O Fundo  é destinado à captação de recursos de investidores pessoas físicas e/ou jurídicas em geral, de Fundos de Investimento, de Fundos de Investimento em Cotas de Fundos de Investimento, das Entidades Fechadas de Previdência Complementar (EFPC) e dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, sujeitos a limites de aplicações estabelecidos pelo administrador, doravante designados, coletivamente, cotistas ou, individualmente, cotista.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa Referenciado DI e investirá, no mínimo, 95% (noventa e cinco por cento) de seus recursos em cotas de fundos de investimento e/ou cotas de fundos de investimento em cotas de fundos de investimento classificados como Renda Fixa Referenciado DI. Os 5% (cinco por cento) remanescentes poderão ser mantidos em depósitos à vista ou aplicados em outros ativos financeiros disponíveis no âmbito do mercado financeiro e de capitais, conforme definido em regulamento.           &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 50.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa Referenciado&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,50 % a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: Até às 17:00h&lt;/b&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Público-alvo e Objetivo&lt;/b&gt; &lt;br&gt;                            
-O fundo é destinado à captação de recursos das Entidades Fechadas de Previdência Privada Complementar (EFPC), dos Regimes Próprios de Previdência Social (RPPS) instituídos pela União, Estados, Distrito Federal e Municípios, das Companhias Seguradoras e de Fundos de Investimento e de Fundos de Investimento em Cotas de Fundos de Investimento, sujeitos a limites de aplicações estabelecidos pelo administrador doravante designados, coletivamente, cotistas ou, individualmente, cotista. O objetivo do fundo é proporcionar aos seus cotistas a valorização de suas cotas por meio da aplicação dos recursos da sua carteira em títulos públicos federais indexados a taxas de juros prefixadas e/ou pós-fixadas (SELIC/CDI), não constituindo, em qualquer hipótese, garantia ou promessa de rentabilidade por parte do administrador.
-&lt;br&gt;&lt;br&gt;
-&lt;b&gt;Política de Investimento&lt;/b&gt;&lt;br&gt;
-O fundo é classificado como Renda Fixa e seus recursos serão aplicados em ativos financeiros e modalidades operacionais disponíveis no âmbito do mercado financeiro e de capitais, observado que a rentabilidade do fundo será impactada pelos custos e despesas do fundo, inclusive taxa de administração. Para alcançar seus objetivos, o fundo aplicará seus recursos exclusivamente em títulos de emissão do Tesouro Nacional, registrados no Sistema Especial de Liquidação e Custódia (SELIC) ou operações compromissadas lastreadas nestes títulos.
-O prazo médio da carteira do fundo será de até 365 (trezentos e sessenta e cinco dias). A carteira do fundo deverá ter como parâmetro de rentabilidade o subíndice IRF-M 1 da ANBIMA          &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100.000,00&lt;/b&gt;&lt;br&gt;                                                              &lt;b&gt;Classificação CVM: Renda Fixa&lt;/b&gt;&lt;br&gt;                                                 &lt;b&gt;Classificação de risco: Baixo &lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 1&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;taxa de administração: 0,15% a.a&lt;/b&gt;&lt;br&gt;                                                                     &lt;b&gt;Horário limite para aplicação e resgate: Até às 16:00h&lt;/b&gt;&lt;br&gt;</t>
+O fundo é classificado como Renda Fixa Curto Prazo e no mínimo 80% (oitenta por cento) da carteira serão aplicados exclusivamente em títulos públicos federais indexados ao CDI/SELIC ou em títulos públicos federais prefixados indexados e/ou sintetizados para CDI/SELIC, e/ou em operações compromissadas lastreadas em títulos públicos federais. Os títulos componentes da carteira deverão ter prazo máximo a decorrer de 375 (trezentos e setenta e cinco) dias, e prazo médio da carteira do fundo inferior a 60 (sessenta) dias.                                                               &lt;br&gt;&lt;br&gt;                                                                                                                  &lt;b&gt;Aplicação inicial: R$ 100,00&lt;/b&gt;&lt;br&gt;  &lt;b&gt;Classificação CVM: Renda Fixa Curto Prazo&lt;/b&gt;&lt;br&gt;                                                                           &lt;b&gt;Classificação de risco: Muito baixo&lt;/b&gt;&lt;br&gt;                                                                        &lt;b&gt;Resgate: D + 0*&lt;/b&gt;&lt;br&gt;                                                                                     &lt;b&gt;Taxa de administração: 1,70% a.a&lt;/b&gt;&lt;br&gt;                                                                      &lt;b&gt;Horário limite para aplicação e resgate: 17:00h&lt;/b&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,49 +599,49 @@
     </row>
     <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>